<commit_message>
Rescale EV power to fix error, ev allocation as tuples
</commit_message>
<xml_diff>
--- a/PRO1/step_3/time_series_example/res_bus/vm_pu.xlsx
+++ b/PRO1/step_3/time_series_example/res_bus/vm_pu.xlsx
@@ -442,61 +442,61 @@
         <v>1.03</v>
       </c>
       <c r="C2">
-        <v>0.9972901753822303</v>
+        <v>1.022287785606226</v>
       </c>
       <c r="D2">
-        <v>0.9877384920205977</v>
+        <v>1.017212861301559</v>
       </c>
       <c r="E2">
-        <v>0.9722441381192682</v>
+        <v>1.008764243556</v>
       </c>
       <c r="F2">
-        <v>0.9713735063161697</v>
+        <v>1.008320882087645</v>
       </c>
       <c r="G2">
-        <v>0.970777596797892</v>
+        <v>1.008018130962079</v>
       </c>
       <c r="H2">
-        <v>0.9700801700342763</v>
+        <v>1.007668345802915</v>
       </c>
       <c r="I2">
-        <v>0.9699202188083061</v>
+        <v>1.007425470330303</v>
       </c>
       <c r="J2">
-        <v>0.9699875801559662</v>
+        <v>1.007462419686843</v>
       </c>
       <c r="K2">
-        <v>0.969594627887546</v>
+        <v>1.007221551487641</v>
       </c>
       <c r="L2">
-        <v>0.9690273796608185</v>
+        <v>1.006920690104309</v>
       </c>
       <c r="M2">
-        <v>0.9689375188854444</v>
+        <v>1.006875393711417</v>
       </c>
       <c r="N2">
-        <v>1.001410718218441</v>
+        <v>1.022734980948664</v>
       </c>
       <c r="O2">
-        <v>0.9997068799377746</v>
+        <v>1.021430049851221</v>
       </c>
       <c r="P2">
-        <v>0.9987174581058191</v>
+        <v>1.02067649724301</v>
       </c>
       <c r="Q2">
-        <v>0.969965227945113</v>
+        <v>1.007446506244054</v>
       </c>
       <c r="R2">
-        <v>0.9996838428809299</v>
+        <v>1.021413915781757</v>
       </c>
       <c r="S2">
-        <v>0.9707552263820419</v>
+        <v>1.008002208741513</v>
       </c>
       <c r="T2">
-        <v>0.9689151908720083</v>
+        <v>1.006859489541038</v>
       </c>
       <c r="U2">
-        <v>0.972221733908712</v>
+        <v>1.008748309550161</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -507,61 +507,61 @@
         <v>1.03</v>
       </c>
       <c r="C3">
-        <v>0.9986362103804298</v>
+        <v>1.022654000256572</v>
       </c>
       <c r="D3">
-        <v>0.9895187342846201</v>
+        <v>1.017826244806614</v>
       </c>
       <c r="E3">
-        <v>0.9747031994276153</v>
+        <v>1.009760920452753</v>
       </c>
       <c r="F3">
-        <v>0.9738694658290185</v>
+        <v>1.009336673118919</v>
       </c>
       <c r="G3">
-        <v>0.9732988806246001</v>
+        <v>1.009047031252258</v>
       </c>
       <c r="H3">
-        <v>0.9726314200779831</v>
+        <v>1.008712747020375</v>
       </c>
       <c r="I3">
-        <v>0.9724814963831446</v>
+        <v>1.008482582963286</v>
       </c>
       <c r="J3">
-        <v>0.9725442189313989</v>
+        <v>1.008516235247874</v>
       </c>
       <c r="K3">
-        <v>0.9721677102998025</v>
+        <v>1.008285332870445</v>
       </c>
       <c r="L3">
-        <v>0.9716243603012932</v>
+        <v>1.007997198739165</v>
       </c>
       <c r="M3">
-        <v>0.9715383740062387</v>
+        <v>1.007953904000022</v>
       </c>
       <c r="N3">
-        <v>1.002524184070991</v>
+        <v>1.023023459945867</v>
       </c>
       <c r="O3">
-        <v>1.000887402362707</v>
+        <v>1.021768915316444</v>
       </c>
       <c r="P3">
-        <v>0.9999365453085443</v>
+        <v>1.021044215156406</v>
       </c>
       <c r="Q3">
-        <v>0.972521807805791</v>
+        <v>1.008500305159468</v>
       </c>
       <c r="R3">
-        <v>1.000864338102124</v>
+        <v>1.021752775894406</v>
       </c>
       <c r="S3">
-        <v>0.9732764521087108</v>
+        <v>1.009031092779627</v>
       </c>
       <c r="T3">
-        <v>0.9715159860591319</v>
+        <v>1.007937982793957</v>
       </c>
       <c r="U3">
-        <v>0.9746807385508685</v>
+        <v>1.009744970703834</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -572,61 +572,61 @@
         <v>1.03</v>
       </c>
       <c r="C4">
-        <v>1.000021328506111</v>
+        <v>1.023030459902508</v>
       </c>
       <c r="D4">
-        <v>0.991350209152595</v>
+        <v>1.018457524838795</v>
       </c>
       <c r="E4">
-        <v>0.9772325097445393</v>
+        <v>1.010787487972367</v>
       </c>
       <c r="F4">
-        <v>0.9764367106198487</v>
+        <v>1.010382957995344</v>
       </c>
       <c r="G4">
-        <v>0.9758921604070564</v>
+        <v>1.010106839194546</v>
       </c>
       <c r="H4">
-        <v>0.9752555058257896</v>
+        <v>1.009788545020354</v>
       </c>
       <c r="I4">
-        <v>0.9751158805280782</v>
+        <v>1.009571488756242</v>
       </c>
       <c r="J4">
-        <v>0.9751738343348062</v>
+        <v>1.00960174003783</v>
       </c>
       <c r="K4">
-        <v>0.9748142286448793</v>
+        <v>1.009381117377024</v>
       </c>
       <c r="L4">
-        <v>0.9742954438460979</v>
+        <v>1.009106111240664</v>
       </c>
       <c r="M4">
-        <v>0.9742134401477196</v>
+        <v>1.009064881190704</v>
       </c>
       <c r="N4">
-        <v>1.003671487913511</v>
+        <v>1.023320448473356</v>
       </c>
       <c r="O4">
-        <v>1.00210385381991</v>
+        <v>1.022117955738541</v>
       </c>
       <c r="P4">
-        <v>1.001192764047728</v>
+        <v>1.021423061652893</v>
       </c>
       <c r="Q4">
-        <v>0.9751513626128372</v>
+        <v>1.009585792803257</v>
       </c>
       <c r="R4">
-        <v>1.00208076152765</v>
+        <v>1.022101810803212</v>
       </c>
       <c r="S4">
-        <v>0.9758696721321169</v>
+        <v>1.010090883981644</v>
       </c>
       <c r="T4">
-        <v>0.974190990556893</v>
+        <v>1.009048942436122</v>
       </c>
       <c r="U4">
-        <v>0.9772099905828421</v>
+        <v>1.01077152200823</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -637,61 +637,61 @@
         <v>1.03</v>
       </c>
       <c r="C5">
-        <v>1.000028267954923</v>
+        <v>1.023032344977129</v>
       </c>
       <c r="D5">
-        <v>0.9913593836921579</v>
+        <v>1.018460687785299</v>
       </c>
       <c r="E5">
-        <v>0.9772451786892096</v>
+        <v>1.010792633532484</v>
       </c>
       <c r="F5">
-        <v>0.9764495695277176</v>
+        <v>1.010388202463306</v>
       </c>
       <c r="G5">
-        <v>0.975905149688099</v>
+        <v>1.010112151498272</v>
       </c>
       <c r="H5">
-        <v>0.9752686493681556</v>
+        <v>1.009793937534579</v>
       </c>
       <c r="I5">
-        <v>0.9751290756140168</v>
+        <v>1.009576947010703</v>
       </c>
       <c r="J5">
-        <v>0.9751870055413338</v>
+        <v>1.009607181232206</v>
       </c>
       <c r="K5">
-        <v>0.9748274844893235</v>
+        <v>1.009386610135802</v>
       </c>
       <c r="L5">
-        <v>0.9743088226941872</v>
+        <v>1.009111669850853</v>
       </c>
       <c r="M5">
-        <v>0.9742268389375519</v>
+        <v>1.009070450157617</v>
       </c>
       <c r="N5">
-        <v>1.003677239748487</v>
+        <v>1.023321936726942</v>
       </c>
       <c r="O5">
-        <v>1.002109952452541</v>
+        <v>1.022119705290602</v>
       </c>
       <c r="P5">
-        <v>1.001199062125959</v>
+        <v>1.021424960830191</v>
       </c>
       <c r="Q5">
-        <v>0.97516453351585</v>
+        <v>1.009591233911687</v>
       </c>
       <c r="R5">
-        <v>1.002086860019744</v>
+        <v>1.022103560327637</v>
       </c>
       <c r="S5">
-        <v>0.975882661113837</v>
+        <v>1.010096196201459</v>
       </c>
       <c r="T5">
-        <v>0.9742043890379665</v>
+        <v>1.00905451131507</v>
       </c>
       <c r="U5">
-        <v>0.9772226592355718</v>
+        <v>1.01077666748707</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -702,61 +702,61 @@
         <v>1.03</v>
       </c>
       <c r="C6">
-        <v>1.000914867588316</v>
+        <v>1.023273096800445</v>
       </c>
       <c r="D6">
-        <v>0.992531450429468</v>
+        <v>1.018864800888</v>
       </c>
       <c r="E6">
-        <v>0.9788635575649791</v>
+        <v>1.01145022836299</v>
       </c>
       <c r="F6">
-        <v>0.9780922114046455</v>
+        <v>1.011058443968311</v>
       </c>
       <c r="G6">
-        <v>0.977564443333263</v>
+        <v>1.010791066721088</v>
       </c>
       <c r="H6">
-        <v>0.9769476456224842</v>
+        <v>1.010483108715772</v>
       </c>
       <c r="I6">
-        <v>0.9768146530448285</v>
+        <v>1.010274522940927</v>
       </c>
       <c r="J6">
-        <v>0.9768695330498532</v>
+        <v>1.010302575830808</v>
       </c>
       <c r="K6">
-        <v>0.9765208218379801</v>
+        <v>1.010088597794501</v>
       </c>
       <c r="L6">
-        <v>0.9760178697874166</v>
+        <v>1.00982207728906</v>
       </c>
       <c r="M6">
-        <v>0.9759384329414672</v>
+        <v>1.009782181811265</v>
       </c>
       <c r="N6">
-        <v>1.004412418302985</v>
+        <v>1.023512101775912</v>
       </c>
       <c r="O6">
-        <v>1.002889468635563</v>
+        <v>1.02234329669413</v>
       </c>
       <c r="P6">
-        <v>1.002004077154457</v>
+        <v>1.021667692889974</v>
       </c>
       <c r="Q6">
-        <v>0.9768470222525228</v>
+        <v>1.010286617526135</v>
       </c>
       <c r="R6">
-        <v>1.002866358239743</v>
+        <v>1.022327148199412</v>
       </c>
       <c r="S6">
-        <v>0.9775419165225511</v>
+        <v>1.010775100700422</v>
       </c>
       <c r="T6">
-        <v>0.9759159436002319</v>
+        <v>1.009766231726512</v>
       </c>
       <c r="U6">
-        <v>0.9788410008177236</v>
+        <v>1.011434251930491</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -767,61 +767,61 @@
         <v>1.03</v>
       </c>
       <c r="C7">
-        <v>1.000223088644751</v>
+        <v>1.023085262169533</v>
       </c>
       <c r="D7">
-        <v>0.9916169486129623</v>
+        <v>1.018549485018173</v>
       </c>
       <c r="E7">
-        <v>0.9776008399696585</v>
+        <v>1.010937099903137</v>
       </c>
       <c r="F7">
-        <v>0.9768105635583022</v>
+        <v>1.010535446088573</v>
       </c>
       <c r="G7">
-        <v>0.9762698036197655</v>
+        <v>1.010261299899466</v>
       </c>
       <c r="H7">
-        <v>0.975637633788958</v>
+        <v>1.009945338182877</v>
       </c>
       <c r="I7">
-        <v>0.9754995068858862</v>
+        <v>1.00973019354211</v>
       </c>
       <c r="J7">
-        <v>0.975556766460796</v>
+        <v>1.009759948731113</v>
       </c>
       <c r="K7">
-        <v>0.9751996213851313</v>
+        <v>1.009540825516052</v>
       </c>
       <c r="L7">
-        <v>0.9746844125728664</v>
+        <v>1.009267734277196</v>
       </c>
       <c r="M7">
-        <v>0.9746029886246805</v>
+        <v>1.009226805391169</v>
       </c>
       <c r="N7">
-        <v>1.003838734176344</v>
+        <v>1.023363719215656</v>
       </c>
       <c r="O7">
-        <v>1.002281184481542</v>
+        <v>1.02216882564266</v>
       </c>
       <c r="P7">
-        <v>1.001375894312373</v>
+        <v>1.021478283003358</v>
       </c>
       <c r="Q7">
-        <v>0.9755342859146112</v>
+        <v>1.009743998997543</v>
       </c>
       <c r="R7">
-        <v>1.002258088102907</v>
+        <v>1.022152679903812</v>
       </c>
       <c r="S7">
-        <v>0.9762473066424868</v>
+        <v>1.010245342246769</v>
       </c>
       <c r="T7">
-        <v>0.9745805300571726</v>
+        <v>1.009210864078903</v>
       </c>
       <c r="U7">
-        <v>0.9775783123202293</v>
+        <v>1.010921131575795</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -832,61 +832,61 @@
         <v>1.03</v>
       </c>
       <c r="C8">
-        <v>0.9985508245369584</v>
+        <v>1.022630780272726</v>
       </c>
       <c r="D8">
-        <v>0.9894058175954611</v>
+        <v>1.01778733211316</v>
       </c>
       <c r="E8">
-        <v>0.9745472416792441</v>
+        <v>1.00969766887615</v>
       </c>
       <c r="F8">
-        <v>0.9737111684463516</v>
+        <v>1.009272207662286</v>
       </c>
       <c r="G8">
-        <v>0.9731389774982291</v>
+        <v>1.008981733264197</v>
       </c>
       <c r="H8">
-        <v>0.9724696169120071</v>
+        <v>1.008646464617772</v>
       </c>
       <c r="I8">
-        <v>0.9723190577006737</v>
+        <v>1.008415493433572</v>
       </c>
       <c r="J8">
-        <v>0.9723820743754207</v>
+        <v>1.008449355101644</v>
       </c>
       <c r="K8">
-        <v>0.9720045231604946</v>
+        <v>1.008217819842967</v>
       </c>
       <c r="L8">
-        <v>0.9714596579477067</v>
+        <v>1.007928877468999</v>
       </c>
       <c r="M8">
-        <v>0.9713734260002533</v>
+        <v>1.007885455614795</v>
       </c>
       <c r="N8">
-        <v>1.002453508224538</v>
+        <v>1.023005156338313</v>
       </c>
       <c r="O8">
-        <v>1.000812468674793</v>
+        <v>1.021747409679758</v>
       </c>
       <c r="P8">
-        <v>0.9998591629035519</v>
+        <v>1.021020875965341</v>
       </c>
       <c r="Q8">
-        <v>0.9723596669862417</v>
+        <v>1.008433426069647</v>
       </c>
       <c r="R8">
-        <v>1.000789406140969</v>
+        <v>1.021731270597415</v>
       </c>
       <c r="S8">
-        <v>0.9731165526671173</v>
+        <v>1.008965795822985</v>
       </c>
       <c r="T8">
-        <v>0.9713510418541774</v>
+        <v>1.007869535489912</v>
       </c>
       <c r="U8">
-        <v>0.9745247843963583</v>
+        <v>1.009681720126326</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -897,61 +897,61 @@
         <v>1.03</v>
       </c>
       <c r="C9">
-        <v>0.9939089825861223</v>
+        <v>1.021363395167066</v>
       </c>
       <c r="D9">
-        <v>0.9832645937986839</v>
+        <v>1.015644861136213</v>
       </c>
       <c r="E9">
-        <v>0.9660620515891098</v>
+        <v>1.006199090528654</v>
       </c>
       <c r="F9">
-        <v>0.9650985798809205</v>
+        <v>1.005707880068399</v>
       </c>
       <c r="G9">
-        <v>0.9644389492921673</v>
+        <v>1.005372312444564</v>
       </c>
       <c r="H9">
-        <v>0.9636661163628544</v>
+        <v>1.00498372247808</v>
       </c>
       <c r="I9">
-        <v>0.9634808885720269</v>
+        <v>1.004698221098066</v>
       </c>
       <c r="J9">
-        <v>0.9635599230865473</v>
+        <v>1.004743428567433</v>
       </c>
       <c r="K9">
-        <v>0.9631255860613008</v>
+        <v>1.004474964022374</v>
       </c>
       <c r="L9">
-        <v>0.9624981892419439</v>
+        <v>1.004135879433539</v>
       </c>
       <c r="M9">
-        <v>0.9623985768582565</v>
+        <v>1.004082849790051</v>
       </c>
       <c r="N9">
-        <v>0.9986201860671033</v>
+        <v>1.022010969472218</v>
       </c>
       <c r="O9">
-        <v>0.9967485149082234</v>
+        <v>1.020580323946099</v>
       </c>
       <c r="P9">
-        <v>0.995662570728837</v>
+        <v>1.019754784223468</v>
       </c>
       <c r="Q9">
-        <v>0.9635377189933592</v>
+        <v>1.004727558072657</v>
       </c>
       <c r="R9">
-        <v>0.996725546023383</v>
+        <v>1.02056420329854</v>
       </c>
       <c r="S9">
-        <v>0.964416724942865</v>
+        <v>1.005356432016209</v>
       </c>
       <c r="T9">
-        <v>0.962376399526912</v>
+        <v>1.003940932901547</v>
       </c>
       <c r="U9">
-        <v>0.9660397898373446</v>
+        <v>1.006183197040868</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -962,61 +962,61 @@
         <v>1.03</v>
       </c>
       <c r="C10">
-        <v>0.977294160382346</v>
+        <v>1.016814234525497</v>
       </c>
       <c r="D10">
-        <v>0.9612346156534075</v>
+        <v>1.008122392769345</v>
       </c>
       <c r="E10">
-        <v>0.9355687675011428</v>
+        <v>0.9940787794780812</v>
       </c>
       <c r="F10">
-        <v>0.9341455607484727</v>
+        <v>0.993356963544071</v>
       </c>
       <c r="G10">
-        <v>0.9331703376582441</v>
+        <v>0.9928632470425405</v>
       </c>
       <c r="H10">
-        <v>0.9320239263308159</v>
+        <v>0.992287637653297</v>
       </c>
       <c r="I10">
-        <v>0.9317125119718371</v>
+        <v>0.9918590550176571</v>
       </c>
       <c r="J10">
-        <v>0.9318493825624278</v>
+        <v>0.9919440492234796</v>
       </c>
       <c r="K10">
-        <v>0.9312098741846546</v>
+        <v>0.9915579309088496</v>
       </c>
       <c r="L10">
-        <v>0.9302842287478458</v>
+        <v>0.9910715578341394</v>
       </c>
       <c r="M10">
-        <v>0.9301362612311664</v>
+        <v>0.9909970864997731</v>
       </c>
       <c r="N10">
-        <v>0.9850484949528674</v>
+        <v>1.018471851288541</v>
       </c>
       <c r="O10">
-        <v>0.9823650073110158</v>
+        <v>1.016441188574724</v>
       </c>
       <c r="P10">
-        <v>0.9808121732392364</v>
+        <v>1.015272061620074</v>
       </c>
       <c r="Q10">
-        <v>0.9318279092009564</v>
+        <v>0.9919283809021914</v>
       </c>
       <c r="R10">
-        <v>0.9823423698770127</v>
+        <v>1.016425133307166</v>
       </c>
       <c r="S10">
-        <v>0.9331488338569327</v>
+        <v>0.992847564201999</v>
       </c>
       <c r="T10">
-        <v>0.9301148273465402</v>
+        <v>0.9909814331363003</v>
       </c>
       <c r="U10">
-        <v>0.9355472084308664</v>
+        <v>0.9940630774375127</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1027,61 +1027,61 @@
         <v>1.03</v>
       </c>
       <c r="C11">
-        <v>0.9619333220416297</v>
+        <v>1.012579261596185</v>
       </c>
       <c r="D11">
-        <v>0.9407882127348668</v>
+        <v>1.001129543381243</v>
       </c>
       <c r="E11">
-        <v>0.907177229907861</v>
+        <v>0.9828381145814358</v>
       </c>
       <c r="F11">
-        <v>0.905322831103369</v>
+        <v>0.9819042122236248</v>
       </c>
       <c r="G11">
-        <v>0.9040515259878814</v>
+        <v>0.9812638691735586</v>
       </c>
       <c r="H11">
-        <v>0.9025544482235447</v>
+        <v>0.9805204341535008</v>
       </c>
       <c r="I11">
-        <v>0.902123018866442</v>
+        <v>0.9799631021533486</v>
       </c>
       <c r="J11">
-        <v>0.9023141857049828</v>
+        <v>0.9800838190276002</v>
       </c>
       <c r="K11">
-        <v>0.9014818564821838</v>
+        <v>0.9795896827800997</v>
       </c>
       <c r="L11">
-        <v>0.9002758300562224</v>
+        <v>0.9789653319239022</v>
       </c>
       <c r="M11">
-        <v>0.9000824018882909</v>
+        <v>0.9788691622574641</v>
       </c>
       <c r="N11">
-        <v>0.9727266526643081</v>
+        <v>1.015240276294989</v>
       </c>
       <c r="O11">
-        <v>0.9693122690085465</v>
+        <v>1.012681064882454</v>
       </c>
       <c r="P11">
-        <v>0.9673390746518535</v>
+        <v>1.011209271566258</v>
       </c>
       <c r="Q11">
-        <v>0.9022933929470189</v>
+        <v>0.9800683380454035</v>
       </c>
       <c r="R11">
-        <v>0.9692899323593838</v>
+        <v>1.012665069008192</v>
       </c>
       <c r="S11">
-        <v>0.9040306931949758</v>
+        <v>0.9811193715294424</v>
       </c>
       <c r="T11">
-        <v>0.9000616605591326</v>
+        <v>0.978853700461463</v>
       </c>
       <c r="U11">
-        <v>0.9071563250868234</v>
+        <v>0.9826937993875077</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1092,61 +1092,61 @@
         <v>1.03</v>
       </c>
       <c r="C12">
-        <v>0.9353286375716811</v>
+        <v>1.005297856383255</v>
       </c>
       <c r="D12">
-        <v>0.9051446806340581</v>
+        <v>0.9893516215900886</v>
       </c>
       <c r="E12">
-        <v>0.8574196211679821</v>
+        <v>0.9641629229935793</v>
       </c>
       <c r="F12">
-        <v>0.8548002877657092</v>
+        <v>0.9628915279497178</v>
       </c>
       <c r="G12">
-        <v>0.8530035094996444</v>
+        <v>0.9620209654525572</v>
       </c>
       <c r="H12">
-        <v>0.8508835916599183</v>
+        <v>0.9609996113219076</v>
       </c>
       <c r="I12">
-        <v>0.8502347438350967</v>
+        <v>0.96020144380735</v>
       </c>
       <c r="J12">
-        <v>0.8505223685802967</v>
+        <v>0.9603813386603203</v>
       </c>
       <c r="K12">
-        <v>0.8493469238686517</v>
+        <v>0.9597081464970401</v>
       </c>
       <c r="L12">
-        <v>0.847641740667301</v>
+        <v>0.9588550439133635</v>
       </c>
       <c r="M12">
-        <v>0.8473673733611456</v>
+        <v>0.9587229041100579</v>
       </c>
       <c r="N12">
-        <v>0.951976021007189</v>
+        <v>1.009783371471103</v>
       </c>
       <c r="O12">
-        <v>0.9473432974888037</v>
+        <v>1.006368473770559</v>
       </c>
       <c r="P12">
-        <v>0.9446693785484562</v>
+        <v>1.004406674851279</v>
       </c>
       <c r="Q12">
-        <v>0.8505027693032015</v>
+        <v>0.9603661688900241</v>
       </c>
       <c r="R12">
-        <v>0.9473214670884783</v>
+        <v>1.006352577607268</v>
       </c>
       <c r="S12">
-        <v>0.8529838530476057</v>
+        <v>0.9620057697834216</v>
       </c>
       <c r="T12">
-        <v>0.8473478467871655</v>
+        <v>0.95870776053568</v>
       </c>
       <c r="U12">
-        <v>0.8573998629518987</v>
+        <v>0.96401639955618</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1157,61 +1157,61 @@
         <v>1.03</v>
       </c>
       <c r="C13">
-        <v>0.9126413533340926</v>
+        <v>0.9992007685579863</v>
       </c>
       <c r="D13">
-        <v>0.8744473575192483</v>
+        <v>0.9795815468474661</v>
       </c>
       <c r="E13">
-        <v>0.8142222590007084</v>
+        <v>0.948786756158456</v>
       </c>
       <c r="F13">
-        <v>0.8109267431689245</v>
+        <v>0.9472342629599226</v>
       </c>
       <c r="G13">
-        <v>0.8086651868026086</v>
+        <v>0.9461697523793638</v>
       </c>
       <c r="H13">
-        <v>0.8059937666231543</v>
+        <v>0.9449247364735041</v>
       </c>
       <c r="I13">
-        <v>0.8051471381436692</v>
+        <v>0.9439498246874815</v>
       </c>
       <c r="J13">
-        <v>0.8055201964276865</v>
+        <v>0.9441773662652847</v>
       </c>
       <c r="K13">
-        <v>0.8040401460142448</v>
+        <v>0.9433599359561322</v>
       </c>
       <c r="L13">
-        <v>0.801891542594341</v>
+        <v>0.9423225294464589</v>
       </c>
       <c r="M13">
-        <v>0.8015452660333942</v>
+        <v>0.9421614112710135</v>
       </c>
       <c r="N13">
-        <v>0.9349798132045726</v>
+        <v>1.005323835672268</v>
       </c>
       <c r="O13">
-        <v>0.9293602066422881</v>
+        <v>1.00123990400822</v>
       </c>
       <c r="P13">
-        <v>0.926118664426504</v>
+        <v>0.9988949779369247</v>
       </c>
       <c r="Q13">
-        <v>0.8055016341721613</v>
+        <v>0.9441624524459624</v>
       </c>
       <c r="R13">
-        <v>0.9293387906409176</v>
+        <v>1.00122408885361</v>
       </c>
       <c r="S13">
-        <v>0.8086465520745181</v>
+        <v>0.9460210073772651</v>
       </c>
       <c r="T13">
-        <v>0.8015267953754153</v>
+        <v>0.9421465292948485</v>
       </c>
       <c r="U13">
-        <v>0.814203496216494</v>
+        <v>0.9487717695311947</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1222,61 +1222,61 @@
         <v>1.03</v>
       </c>
       <c r="C14">
-        <v>0.9104523071903119</v>
+        <v>0.9986215517192463</v>
       </c>
       <c r="D14">
-        <v>0.8714673454339197</v>
+        <v>0.9786578776209675</v>
       </c>
       <c r="E14">
-        <v>0.8100082817070896</v>
+        <v>0.9473385853787518</v>
       </c>
       <c r="F14">
-        <v>0.8066460872250381</v>
+        <v>0.9457603423155501</v>
       </c>
       <c r="G14">
-        <v>0.804338683368704</v>
+        <v>0.9446781772519762</v>
       </c>
       <c r="H14">
-        <v>0.8016128265724511</v>
+        <v>0.943412280980801</v>
       </c>
       <c r="I14">
-        <v>0.8007463741133046</v>
+        <v>0.9424198641885545</v>
       </c>
       <c r="J14">
-        <v>0.8011278665939083</v>
+        <v>0.9426518552720584</v>
       </c>
       <c r="K14">
-        <v>0.7996177043408017</v>
+        <v>0.9418209512915393</v>
       </c>
       <c r="L14">
-        <v>0.797425250175805</v>
+        <v>0.9407663268951646</v>
       </c>
       <c r="M14">
-        <v>0.7970718619086483</v>
+        <v>0.9406025016556544</v>
       </c>
       <c r="N14">
-        <v>0.9333789452217714</v>
+        <v>1.004905102963169</v>
       </c>
       <c r="O14">
-        <v>0.9276668715757515</v>
+        <v>1.000759622930117</v>
       </c>
       <c r="P14">
-        <v>0.9243721442861793</v>
+        <v>0.9983794504093206</v>
       </c>
       <c r="Q14">
-        <v>0.8011094055544036</v>
+        <v>0.9426369655490513</v>
       </c>
       <c r="R14">
-        <v>0.9276454945952749</v>
+        <v>1.000743815361821</v>
       </c>
       <c r="S14">
-        <v>0.804320148339743</v>
+        <v>0.944529243781845</v>
       </c>
       <c r="T14">
-        <v>0.7970534943349508</v>
+        <v>0.9405876443033552</v>
       </c>
       <c r="U14">
-        <v>0.8099896160289731</v>
+        <v>0.9473236216261729</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1287,61 +1287,61 @@
         <v>1.03</v>
       </c>
       <c r="C15">
-        <v>0.9122355974903252</v>
+        <v>0.9990932648265023</v>
       </c>
       <c r="D15">
-        <v>0.8738952544989456</v>
+        <v>0.9794100578919419</v>
       </c>
       <c r="E15">
-        <v>0.8134418386132896</v>
+        <v>0.9485178203192088</v>
       </c>
       <c r="F15">
-        <v>0.8101339843824195</v>
+        <v>0.9469605423227835</v>
       </c>
       <c r="G15">
-        <v>0.8078639444925867</v>
+        <v>0.9458927512012324</v>
       </c>
       <c r="H15">
-        <v>0.8051824519646303</v>
+        <v>0.9446438553476416</v>
       </c>
       <c r="I15">
-        <v>0.8043321597947414</v>
+        <v>0.9436656915825906</v>
       </c>
       <c r="J15">
-        <v>0.8047067786287428</v>
+        <v>0.9438940599440638</v>
       </c>
       <c r="K15">
-        <v>0.803221157304952</v>
+        <v>0.9430741260810747</v>
       </c>
       <c r="L15">
-        <v>0.8010644414107111</v>
+        <v>0.9420335203224284</v>
       </c>
       <c r="M15">
-        <v>0.8007168491765323</v>
+        <v>0.9418718991467286</v>
       </c>
       <c r="N15">
-        <v>0.9346825269768807</v>
+        <v>1.005246053913137</v>
       </c>
       <c r="O15">
-        <v>0.9290457427805855</v>
+        <v>1.001150673458975</v>
       </c>
       <c r="P15">
-        <v>0.9257943203731009</v>
+        <v>0.9987991910979196</v>
       </c>
       <c r="Q15">
-        <v>0.8046882351174638</v>
+        <v>0.9438791505997262</v>
       </c>
       <c r="R15">
-        <v>0.9290243340256606</v>
+        <v>1.001134859713812</v>
       </c>
       <c r="S15">
-        <v>0.807845328228173</v>
+        <v>0.945743971249475</v>
       </c>
       <c r="T15">
-        <v>0.8006983976084352</v>
+        <v>0.9418570217435728</v>
       </c>
       <c r="U15">
-        <v>0.8134230938129356</v>
+        <v>0.9485028379399425</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1352,61 +1352,61 @@
         <v>1.03</v>
       </c>
       <c r="C16">
-        <v>0.9122890425092536</v>
+        <v>0.9991154903043679</v>
       </c>
       <c r="D16">
-        <v>0.8739679827258184</v>
+        <v>0.9794698238863061</v>
       </c>
       <c r="E16">
-        <v>0.8135446505948375</v>
+        <v>0.9486338037481729</v>
       </c>
       <c r="F16">
-        <v>0.8102384220808536</v>
+        <v>0.9470826784383699</v>
       </c>
       <c r="G16">
-        <v>0.80796949999223</v>
+        <v>0.9460203364731335</v>
       </c>
       <c r="H16">
-        <v>0.8052893346238824</v>
+        <v>0.9447720817729454</v>
       </c>
       <c r="I16">
-        <v>0.8044395253022947</v>
+        <v>0.9437841314117045</v>
       </c>
       <c r="J16">
-        <v>0.8048139385135337</v>
+        <v>0.9440123636415927</v>
       </c>
       <c r="K16">
-        <v>0.803329051244481</v>
+        <v>0.9431928329934556</v>
       </c>
       <c r="L16">
-        <v>0.8011734043018592</v>
+        <v>0.9421527429998072</v>
       </c>
       <c r="M16">
-        <v>0.8008259854293848</v>
+        <v>0.9419912030542555</v>
       </c>
       <c r="N16">
-        <v>0.9347216704358825</v>
+        <v>1.005256294824117</v>
       </c>
       <c r="O16">
-        <v>0.9290871478440935</v>
+        <v>1.001162421326962</v>
       </c>
       <c r="P16">
-        <v>0.9258370262613882</v>
+        <v>0.9988118019433887</v>
       </c>
       <c r="Q16">
-        <v>0.8047953925328826</v>
+        <v>0.943997452428581</v>
       </c>
       <c r="R16">
-        <v>0.9290657381350381</v>
+        <v>1.001146607396236</v>
       </c>
       <c r="S16">
-        <v>0.8079508812954149</v>
+        <v>0.9460053935431979</v>
       </c>
       <c r="T16">
-        <v>0.8008075313463725</v>
+        <v>0.9419763237666264</v>
       </c>
       <c r="U16">
-        <v>0.8135259034253033</v>
+        <v>0.9486188195368824</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1417,61 +1417,61 @@
         <v>1.03</v>
       </c>
       <c r="C17">
-        <v>0.9125209632011567</v>
+        <v>0.9991685450904111</v>
       </c>
       <c r="D17">
-        <v>0.8742835577265511</v>
+        <v>0.9795298811143368</v>
       </c>
       <c r="E17">
-        <v>0.8139907352255116</v>
+        <v>0.9487054610845316</v>
       </c>
       <c r="F17">
-        <v>0.8106915595035672</v>
+        <v>0.947156925170781</v>
       </c>
       <c r="G17">
-        <v>0.8084274867138641</v>
+        <v>0.9460963582884252</v>
       </c>
       <c r="H17">
-        <v>0.8057530788491383</v>
+        <v>0.9448502033189333</v>
       </c>
       <c r="I17">
-        <v>0.8049053638395152</v>
+        <v>0.9438523826731062</v>
       </c>
       <c r="J17">
-        <v>0.805278885016831</v>
+        <v>0.9440801740668923</v>
       </c>
       <c r="K17">
-        <v>0.8037971821765652</v>
+        <v>0.9432591592803155</v>
       </c>
       <c r="L17">
-        <v>0.8016461724696962</v>
+        <v>0.9422139971591037</v>
       </c>
       <c r="M17">
-        <v>0.8012995056597629</v>
+        <v>0.9420498245984484</v>
       </c>
       <c r="N17">
-        <v>0.934891580559715</v>
+        <v>1.005300749529178</v>
       </c>
       <c r="O17">
-        <v>0.9292668754900186</v>
+        <v>1.0012134190303</v>
       </c>
       <c r="P17">
-        <v>0.9260224007271902</v>
+        <v>0.9988665465748486</v>
       </c>
       <c r="Q17">
-        <v>0.8052603283220404</v>
+        <v>0.9440652617827765</v>
       </c>
       <c r="R17">
-        <v>0.9292454616393534</v>
+        <v>1.001197604294035</v>
       </c>
       <c r="S17">
-        <v>0.8084088574632897</v>
+        <v>0.946081414157531</v>
       </c>
       <c r="T17">
-        <v>0.8012810406650398</v>
+        <v>0.941900557379894</v>
       </c>
       <c r="U17">
-        <v>0.813971977776487</v>
+        <v>0.9486904757413724</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1482,61 +1482,61 @@
         <v>1.03</v>
       </c>
       <c r="C18">
-        <v>0.9343421576066683</v>
+        <v>1.005036260194141</v>
       </c>
       <c r="D18">
-        <v>0.9038163521460927</v>
+        <v>0.9889541967628399</v>
       </c>
       <c r="E18">
-        <v>0.8555576789196995</v>
+        <v>0.9635569414156528</v>
       </c>
       <c r="F18">
-        <v>0.8529094541598409</v>
+        <v>0.9622733393025414</v>
       </c>
       <c r="G18">
-        <v>0.8510928227983683</v>
+        <v>0.9613944074160036</v>
       </c>
       <c r="H18">
-        <v>0.8489493596909797</v>
+        <v>0.9603631525905185</v>
       </c>
       <c r="I18">
-        <v>0.848292175435892</v>
+        <v>0.9595567316133728</v>
       </c>
       <c r="J18">
-        <v>0.8485834471066804</v>
+        <v>0.9597387327633737</v>
       </c>
       <c r="K18">
-        <v>0.8473950140102501</v>
+        <v>0.9590591572655405</v>
       </c>
       <c r="L18">
-        <v>0.8456709292045793</v>
+        <v>0.9581978993226578</v>
       </c>
       <c r="M18">
-        <v>0.8453934967942596</v>
+        <v>0.9580644773226147</v>
       </c>
       <c r="N18">
-        <v>0.9512226318330947</v>
+        <v>1.009585311052824</v>
       </c>
       <c r="O18">
-        <v>0.9465459581379562</v>
+        <v>1.006140152316456</v>
       </c>
       <c r="P18">
-        <v>0.9438467608753383</v>
+        <v>1.004161024335809</v>
       </c>
       <c r="Q18">
-        <v>0.8485638925097261</v>
+        <v>0.9597235731434036</v>
       </c>
       <c r="R18">
-        <v>0.9465241461113685</v>
+        <v>1.006124259759633</v>
       </c>
       <c r="S18">
-        <v>0.8510732103758338</v>
+        <v>0.9613792216437091</v>
       </c>
       <c r="T18">
-        <v>0.8453740157059187</v>
+        <v>0.9580493441484635</v>
       </c>
       <c r="U18">
-        <v>0.8555379636098623</v>
+        <v>0.9635417214849021</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -1547,61 +1547,61 @@
         <v>1.03</v>
       </c>
       <c r="C19">
-        <v>0.9694545709257349</v>
+        <v>1.014644825834384</v>
       </c>
       <c r="D19">
-        <v>0.9508100665337906</v>
+        <v>1.0044859306647</v>
       </c>
       <c r="E19">
-        <v>0.9211053885724043</v>
+        <v>0.9881818418478231</v>
       </c>
       <c r="F19">
-        <v>0.9194629396627478</v>
+        <v>0.9873535109780535</v>
       </c>
       <c r="G19">
-        <v>0.918337182482894</v>
+        <v>0.9867867509051887</v>
       </c>
       <c r="H19">
-        <v>0.9170125085166407</v>
+        <v>0.9861247533970452</v>
       </c>
       <c r="I19">
-        <v>0.9166402836586713</v>
+        <v>0.9856027626734759</v>
       </c>
       <c r="J19">
-        <v>0.916804755047236</v>
+        <v>0.9857061536823657</v>
       </c>
       <c r="K19">
-        <v>0.9160672551526022</v>
+        <v>0.985259026330925</v>
       </c>
       <c r="L19">
-        <v>0.9149991310534912</v>
+        <v>0.9846886414928995</v>
       </c>
       <c r="M19">
-        <v>0.9148280625139689</v>
+        <v>0.9845974429970322</v>
       </c>
       <c r="N19">
-        <v>0.9787312543702411</v>
+        <v>1.016814662975463</v>
       </c>
       <c r="O19">
-        <v>0.9756723314261947</v>
+        <v>1.014470401983127</v>
       </c>
       <c r="P19">
-        <v>0.9739035743352553</v>
+        <v>1.013144948709212</v>
       </c>
       <c r="Q19">
-        <v>0.9167836283713245</v>
+        <v>0.9856905838921906</v>
       </c>
       <c r="R19">
-        <v>0.9756498482169527</v>
+        <v>1.014329615859043</v>
       </c>
       <c r="S19">
-        <v>0.9183160204940136</v>
+        <v>0.9867711640463649</v>
       </c>
       <c r="T19">
-        <v>0.9148069813885875</v>
+        <v>0.9843243399380063</v>
       </c>
       <c r="U19">
-        <v>0.9210841627935046</v>
+        <v>0.9880381410241772</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -1612,61 +1612,61 @@
         <v>1.03</v>
       </c>
       <c r="C20">
-        <v>0.9780755826989778</v>
+        <v>1.017021268077087</v>
       </c>
       <c r="D20">
-        <v>0.9622725757830048</v>
+        <v>1.008417848860809</v>
       </c>
       <c r="E20">
-        <v>0.9370075928254195</v>
+        <v>0.9945116483922374</v>
       </c>
       <c r="F20">
-        <v>0.9356061519461873</v>
+        <v>0.9938004062075536</v>
       </c>
       <c r="G20">
-        <v>0.9346458723900771</v>
+        <v>0.9933139407192726</v>
       </c>
       <c r="H20">
-        <v>0.9335171546709846</v>
+        <v>0.9927469055560827</v>
       </c>
       <c r="I20">
-        <v>0.9332117543595144</v>
+        <v>0.9923144417915316</v>
       </c>
       <c r="J20">
-        <v>0.9333458855102319</v>
+        <v>0.9923976180917748</v>
       </c>
       <c r="K20">
-        <v>0.9327161001300371</v>
+        <v>0.9920143350349426</v>
       </c>
       <c r="L20">
-        <v>0.9318045906434017</v>
+        <v>0.9915285654837306</v>
       </c>
       <c r="M20">
-        <v>0.9316589150500842</v>
+        <v>0.9914524451902142</v>
       </c>
       <c r="N20">
-        <v>0.985681324299656</v>
+        <v>1.018637431352431</v>
       </c>
       <c r="O20">
-        <v>0.9830355300567426</v>
+        <v>1.016634328864176</v>
       </c>
       <c r="P20">
-        <v>0.9815043743525037</v>
+        <v>1.015480983800037</v>
       </c>
       <c r="Q20">
-        <v>0.9333243776636289</v>
+        <v>0.9923819426061079</v>
       </c>
       <c r="R20">
-        <v>0.9830128771713398</v>
+        <v>1.016618270545856</v>
       </c>
       <c r="S20">
-        <v>0.9346243345868216</v>
+        <v>0.9932982507597676</v>
       </c>
       <c r="T20">
-        <v>0.9316374460777106</v>
+        <v>0.991309116654614</v>
       </c>
       <c r="U20">
-        <v>0.9369860005991236</v>
+        <v>0.9943686655449495</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -1677,61 +1677,61 @@
         <v>1.03</v>
       </c>
       <c r="C21">
-        <v>0.9870717572737202</v>
+        <v>1.019493935132369</v>
       </c>
       <c r="D21">
-        <v>0.9742085840411447</v>
+        <v>1.01253269180433</v>
       </c>
       <c r="E21">
-        <v>0.9535379142579465</v>
+        <v>1.00116330884761</v>
       </c>
       <c r="F21">
-        <v>0.9523860002815978</v>
+        <v>1.000571246704534</v>
       </c>
       <c r="G21">
-        <v>0.9515970210149075</v>
+        <v>1.00016534495993</v>
       </c>
       <c r="H21">
-        <v>0.9506710964963522</v>
+        <v>0.9996990672186851</v>
       </c>
       <c r="I21">
-        <v>0.9504343552007153</v>
+        <v>0.999370229859364</v>
       </c>
       <c r="J21">
-        <v>0.9505370898593712</v>
+        <v>0.9994319618082639</v>
       </c>
       <c r="K21">
-        <v>0.9500187033478775</v>
+        <v>0.999116185211681</v>
       </c>
       <c r="L21">
-        <v>0.9492691382752334</v>
+        <v>0.9987196546569652</v>
       </c>
       <c r="M21">
-        <v>0.9491497190225276</v>
+        <v>0.9986593122481833</v>
       </c>
       <c r="N21">
-        <v>0.9930062950025175</v>
+        <v>1.020550319408322</v>
       </c>
       <c r="O21">
-        <v>0.9907979349814863</v>
+        <v>1.01886919354919</v>
       </c>
       <c r="P21">
-        <v>0.9895183563982752</v>
+        <v>1.017900222117251</v>
       </c>
       <c r="Q21">
-        <v>0.9505151858618964</v>
+        <v>0.999416175211131</v>
       </c>
       <c r="R21">
-        <v>0.9907751032206877</v>
+        <v>1.01885309992991</v>
       </c>
       <c r="S21">
-        <v>0.9515750925925792</v>
+        <v>1.000022994602922</v>
       </c>
       <c r="T21">
-        <v>0.949127846995365</v>
+        <v>0.9986435378554902</v>
       </c>
       <c r="U21">
-        <v>0.9535159411100405</v>
+        <v>1.001147494902864</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -1742,61 +1742,61 @@
         <v>1.03</v>
       </c>
       <c r="C22">
-        <v>0.9903379090214885</v>
+        <v>1.020387907091106</v>
       </c>
       <c r="D22">
-        <v>0.9785362350552477</v>
+        <v>1.014018869207036</v>
       </c>
       <c r="E22">
-        <v>0.9595246983788731</v>
+        <v>1.003565790772829</v>
       </c>
       <c r="F22">
-        <v>0.9584629256488959</v>
+        <v>1.003019350018149</v>
       </c>
       <c r="G22">
-        <v>0.9577358220259488</v>
+        <v>1.002644738489521</v>
       </c>
       <c r="H22">
-        <v>0.9568831347998061</v>
+        <v>1.002215448490336</v>
       </c>
       <c r="I22">
-        <v>0.9566710702798789</v>
+        <v>1.001916990819399</v>
       </c>
       <c r="J22">
-        <v>0.956762466893317</v>
+        <v>1.001970853808667</v>
       </c>
       <c r="K22">
-        <v>0.9562842936400376</v>
+        <v>1.001678866124234</v>
       </c>
       <c r="L22">
-        <v>0.955593181473722</v>
+        <v>1.00131271818597</v>
       </c>
       <c r="M22">
-        <v>0.9554832391131597</v>
+        <v>1.001257153995579</v>
       </c>
       <c r="N22">
-        <v>0.9956831528935083</v>
+        <v>1.021247445476572</v>
       </c>
       <c r="O22">
-        <v>0.9936351779708075</v>
+        <v>1.019685351916267</v>
       </c>
       <c r="P22">
-        <v>0.9924478392875624</v>
+        <v>1.018784541653293</v>
       </c>
       <c r="Q22">
-        <v>0.956740419439428</v>
+        <v>1.001955027108289</v>
       </c>
       <c r="R22">
-        <v>0.9936122808291167</v>
+        <v>1.019669245405301</v>
       </c>
       <c r="S22">
-        <v>0.9577137521422474</v>
+        <v>1.002502662927118</v>
       </c>
       <c r="T22">
-        <v>0.9554612211375542</v>
+        <v>1.001241338568496</v>
       </c>
       <c r="U22">
-        <v>0.9595025872726424</v>
+        <v>1.003549938879513</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -1807,61 +1807,61 @@
         <v>1.03</v>
       </c>
       <c r="C23">
-        <v>0.9914381621724526</v>
+        <v>1.020691703352726</v>
       </c>
       <c r="D23">
-        <v>0.9799934111781675</v>
+        <v>1.01454752307477</v>
       </c>
       <c r="E23">
-        <v>0.9615397773903057</v>
+        <v>1.004442181352812</v>
       </c>
       <c r="F23">
-        <v>0.9605083192236545</v>
+        <v>1.003916258241095</v>
       </c>
       <c r="G23">
-        <v>0.9598020236849574</v>
+        <v>1.00355688396569</v>
       </c>
       <c r="H23">
-        <v>0.9589739637171284</v>
+        <v>1.003140143366839</v>
       </c>
       <c r="I23">
-        <v>0.9587701833832989</v>
+        <v>1.002842309368001</v>
       </c>
       <c r="J23">
-        <v>0.9588577674576804</v>
+        <v>1.002893501435303</v>
       </c>
       <c r="K23">
-        <v>0.9583931145391261</v>
+        <v>1.002609580027543</v>
       </c>
       <c r="L23">
-        <v>0.9577216544113054</v>
+        <v>1.002253734394235</v>
       </c>
       <c r="M23">
-        <v>0.9576148981883276</v>
+        <v>1.002199790564773</v>
       </c>
       <c r="N23">
-        <v>0.9965869249183255</v>
+        <v>1.021482550812523</v>
       </c>
       <c r="O23">
-        <v>0.9945931645277498</v>
+        <v>1.019960811448615</v>
       </c>
       <c r="P23">
-        <v>0.9934370053525293</v>
+        <v>1.019083109065594</v>
       </c>
       <c r="Q23">
-        <v>0.9588356717200799</v>
+        <v>1.00287766016118</v>
       </c>
       <c r="R23">
-        <v>0.9945702453103972</v>
+        <v>1.019944700586609</v>
       </c>
       <c r="S23">
-        <v>0.9597799061880946</v>
+        <v>1.00354103221437</v>
       </c>
       <c r="T23">
-        <v>0.9575928310911724</v>
+        <v>1.002183960248208</v>
       </c>
       <c r="U23">
-        <v>0.9615176198489741</v>
+        <v>1.004426315616407</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -1872,61 +1872,61 @@
         <v>1.03</v>
       </c>
       <c r="C24">
-        <v>0.9941441073711104</v>
+        <v>1.02143047738283</v>
       </c>
       <c r="D24">
-        <v>0.9835757983632857</v>
+        <v>1.015779633355027</v>
       </c>
       <c r="E24">
-        <v>0.9664921845930272</v>
+        <v>1.006438391812122</v>
       </c>
       <c r="F24">
-        <v>0.9655351761144836</v>
+        <v>1.005950535740439</v>
       </c>
       <c r="G24">
-        <v>0.9648799817005643</v>
+        <v>1.005617268730074</v>
       </c>
       <c r="H24">
-        <v>0.9641123986865929</v>
+        <v>1.00523139969446</v>
       </c>
       <c r="I24">
-        <v>0.963928932734096</v>
+        <v>1.004958916346667</v>
       </c>
       <c r="J24">
-        <v>0.9640071545311557</v>
+        <v>1.005003541199729</v>
       </c>
       <c r="K24">
-        <v>0.9635756990898372</v>
+        <v>1.004739471894131</v>
       </c>
       <c r="L24">
-        <v>0.962952490475288</v>
+        <v>1.004408980128753</v>
       </c>
       <c r="M24">
-        <v>0.9628535571087118</v>
+        <v>1.004359023710278</v>
       </c>
       <c r="N24">
-        <v>0.9988139352398119</v>
+        <v>1.022061284486923</v>
       </c>
       <c r="O24">
-        <v>0.996953906655928</v>
+        <v>1.020639341486578</v>
       </c>
       <c r="P24">
-        <v>0.9958746582504339</v>
+        <v>1.019818785046902</v>
       </c>
       <c r="Q24">
-        <v>0.9639849401320507</v>
+        <v>1.004987666596326</v>
       </c>
       <c r="R24">
-        <v>0.9969309330380789</v>
+        <v>1.020623219906803</v>
       </c>
       <c r="S24">
-        <v>0.9648577471881945</v>
+        <v>1.005601384432494</v>
       </c>
       <c r="T24">
-        <v>0.962831369292888</v>
+        <v>1.004343159287396</v>
       </c>
       <c r="U24">
-        <v>0.9664699129293579</v>
+        <v>1.006422494544436</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -1937,61 +1937,61 @@
         <v>1.03</v>
       </c>
       <c r="C25">
-        <v>0.9953516277359779</v>
+        <v>1.021759745374283</v>
       </c>
       <c r="D25">
-        <v>0.9851738147499727</v>
+        <v>1.016329653648021</v>
       </c>
       <c r="E25">
-        <v>0.9687006375036022</v>
+        <v>1.00733047989036</v>
       </c>
       <c r="F25">
-        <v>0.9677768047582833</v>
+        <v>1.00685967173793</v>
       </c>
       <c r="G25">
-        <v>0.9671443809547386</v>
+        <v>1.006538096703128</v>
       </c>
       <c r="H25">
-        <v>0.9664037448633458</v>
+        <v>1.006166053090969</v>
       </c>
       <c r="I25">
-        <v>0.9662293173087234</v>
+        <v>1.005904916820103</v>
       </c>
       <c r="J25">
-        <v>0.9663033675893302</v>
+        <v>1.005946600764998</v>
       </c>
       <c r="K25">
-        <v>0.9658867021154064</v>
+        <v>1.005691421245162</v>
       </c>
       <c r="L25">
-        <v>0.9652849895438352</v>
+        <v>1.005372282800053</v>
       </c>
       <c r="M25">
-        <v>0.9651895412383495</v>
+        <v>1.005324111933676</v>
       </c>
       <c r="N25">
-        <v>0.999809678026633</v>
+        <v>1.022319763117535</v>
       </c>
       <c r="O25">
-        <v>0.9980095085873909</v>
+        <v>1.0209426063822</v>
       </c>
       <c r="P25">
-        <v>0.9969646858064563</v>
+        <v>1.020147695657129</v>
       </c>
       <c r="Q25">
-        <v>0.9662811002767241</v>
+        <v>1.005930711265432</v>
       </c>
       <c r="R25">
-        <v>0.9979865106444501</v>
+        <v>1.020926480012183</v>
       </c>
       <c r="S25">
-        <v>0.9671220942619793</v>
+        <v>1.006522197860547</v>
       </c>
       <c r="T25">
-        <v>0.9651672995925481</v>
+        <v>1.005308232266676</v>
       </c>
       <c r="U25">
-        <v>0.9686783149487603</v>
+        <v>1.007314568531635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>